<commit_message>
collected papers to read
</commit_message>
<xml_diff>
--- a/CAS_papers.xlsx
+++ b/CAS_papers.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20371"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_F25DC773A252ABEACE02EC5EFB1E560C5ADE58A3" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{3284A68E-E1F5-498E-BE8D-A2565FD4C5FE}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="11_F25DC773A252ABEACE02EC5EFB1E560C5ADE58A3" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{50DF9488-887B-4D51-B366-F04FE5319405}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>Name</t>
   </si>
@@ -43,37 +43,73 @@
     <t>Flexible Models for Microclustering with Application to Entity Resolution</t>
   </si>
   <si>
-    <t>https://arxiv.org/abs/1610.09780</t>
-  </si>
-  <si>
-    <t>Framework for Evaluating Clustering Algorithms in Duplicate Detection</t>
-  </si>
-  <si>
-    <t>http://dblab.cs.toronto.edu/~fchiang/docs/vldb09.pdf</t>
-  </si>
-  <si>
-    <t>Handbook of Cluster Analysis</t>
-  </si>
-  <si>
-    <t>https://sites.stat.washington.edu/people/mmp/Papers/ch2.2.pdf</t>
-  </si>
-  <si>
     <t>A Hierarchical Algorithm for Extreme Clustering</t>
   </si>
   <si>
-    <t>https://dl.acm.org/doi/pdf/10.1145/3097983.3098079</t>
-  </si>
-  <si>
-    <t>Dimension Independent Similarity Computation</t>
-  </si>
-  <si>
-    <t>https://www.jmlr.org/papers/volume14/bosagh-zadeh13a/bosagh-zadeh13a.pdf</t>
-  </si>
-  <si>
-    <t>Efficient Edit Similarity Joins via Embeddings</t>
-  </si>
-  <si>
-    <t>https://arxiv.org/abs/1702.00093</t>
+    <t>Low Distortion Embeddings for Edit Distance</t>
+  </si>
+  <si>
+    <t>https://citeseerx.ist.psu.edu/viewdoc/download?doi=10.1.1.1077.3119&amp;rep=rep1&amp;type=pdf</t>
+  </si>
+  <si>
+    <t>A Comprehensive Survey of Clustering Algorithms</t>
+  </si>
+  <si>
+    <t>https://link.springer.com/article/10.1007/s40745-015-0040-1</t>
+  </si>
+  <si>
+    <t>Survey of Clustering Algorithms</t>
+  </si>
+  <si>
+    <t>https://scholarsmine.mst.edu/cgi/viewcontent.cgi?article=1763&amp;context=ele_comeng_facwork</t>
+  </si>
+  <si>
+    <t>A Characterization of the DNA Data Storage Channel</t>
+  </si>
+  <si>
+    <t>https://www.nature.com/articles/s41598-019-45832-6#Sec7</t>
+  </si>
+  <si>
+    <t>https://papers.nips.cc/paper/2016/file/670e8a43b246801ca1eaca97b3e19189-Paper.pdf</t>
+  </si>
+  <si>
+    <t>https://dl.acm.org/doi/abs/10.1145/3097983.3098079</t>
+  </si>
+  <si>
+    <t>EmbedJoin: Efficient Edit Similarity Joins via Embeddings</t>
+  </si>
+  <si>
+    <t>https://dl.acm.org/doi/abs/10.1145/3097983.3098003</t>
+  </si>
+  <si>
+    <t>Convolutional Embedding for Edit Distance</t>
+  </si>
+  <si>
+    <t>https://arxiv.org/abs/2001.11692</t>
+  </si>
+  <si>
+    <t>Deep metric learning using Triplet network</t>
+  </si>
+  <si>
+    <t>https://arxiv.org/abs/1412.6622</t>
+  </si>
+  <si>
+    <t>http://proceedings.mlr.press/v48/xieb16.html</t>
+  </si>
+  <si>
+    <t>Unsupervised Deep Embedding for Clustering Analysis</t>
+  </si>
+  <si>
+    <t>Clustering with Deep Learning: Taxonomy and New Methods</t>
+  </si>
+  <si>
+    <t>https://arxiv.org/abs/1801.07648</t>
+  </si>
+  <si>
+    <t>A Survey of Clustering With Deep Learning: From the Perspective of Network Architecture</t>
+  </si>
+  <si>
+    <t>https://ieeexplore.ieee.org/abstract/document/8412085</t>
   </si>
 </sst>
 </file>
@@ -406,10 +442,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A15" sqref="A15:XFD15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -425,11 +461,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
     </row>
@@ -443,10 +479,10 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -473,20 +509,68 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="8" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" t="s">
         <v>16</v>
       </c>
-      <c r="B9" t="s">
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" t="s">
         <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>